<commit_message>
reveral report, tabbed, table - norms
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/rhme_sum-raw-ss-lookup.xlsx
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,222 +376,242 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>82</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>110</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B13">
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
         <v>112</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>113</v>
-      </c>
-    </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>115</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="B16">
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>117</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="B17">
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>119</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B18">
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>121</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="B19">
-        <v>122</v>
-      </c>
-    </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>124</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B21">
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
         <v>126</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B22">
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
         <v>128</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>23 - 30</t>
-        </is>
-      </c>
-      <c r="B23">
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
         <v>130</v>
       </c>
     </row>
@@ -602,7 +622,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -633,214 +653,230 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>130</v>
       </c>
     </row>
@@ -851,7 +887,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -870,242 +906,242 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1 - 7</t>
-        </is>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>88</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B4">
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>90</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B5">
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>91</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B6">
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>93</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B7">
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>94</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B8">
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
         <v>96</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B9">
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
         <v>97</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B10">
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>99</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="B11">
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>100</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="B12">
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>102</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B13">
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>103</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="B14">
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>105</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B15">
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>107</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B16">
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
         <v>108</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B17">
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
         <v>110</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B18">
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
         <v>112</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="B19">
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
         <v>114</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="B20">
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
         <v>116</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="B21">
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
         <v>118</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="B22">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B23">
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
         <v>123</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="B25">
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
         <v>130</v>
       </c>
     </row>
@@ -1139,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -1171,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -1187,7 +1223,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
@@ -1363,7 +1399,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -1404,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -1412,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -1420,7 +1456,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -1436,7 +1472,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
@@ -1452,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
@@ -1460,7 +1496,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10">
@@ -1484,7 +1520,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
@@ -1508,7 +1544,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -1532,7 +1568,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -1548,7 +1584,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1628,7 +1664,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
@@ -1669,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -1677,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
@@ -1685,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -1693,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -1701,7 +1737,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
@@ -1709,7 +1745,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
@@ -1717,7 +1753,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
@@ -1725,7 +1761,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -1733,7 +1769,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
@@ -1741,7 +1777,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
@@ -1749,7 +1785,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
@@ -1765,7 +1801,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
@@ -1773,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -1781,7 +1817,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -1797,7 +1833,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -1813,7 +1849,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -1829,7 +1865,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -1837,7 +1873,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
@@ -1845,7 +1881,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25">
@@ -1853,7 +1889,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -1877,7 +1913,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29">
@@ -1885,7 +1921,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -1934,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
@@ -1942,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -1950,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -1958,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -1966,7 +2002,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
@@ -1974,7 +2010,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -1982,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -1990,7 +2026,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
@@ -1998,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -2006,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -2014,7 +2050,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -2022,7 +2058,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -2030,7 +2066,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -2038,7 +2074,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -2046,7 +2082,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -2054,7 +2090,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -2062,7 +2098,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -2070,7 +2106,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -2078,7 +2114,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -2094,7 +2130,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23">
@@ -2102,7 +2138,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24">
@@ -2118,7 +2154,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26">
@@ -2134,7 +2170,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28">
@@ -2142,7 +2178,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">

</xml_diff>